<commit_message>
JDAP adoption dates updated.
</commit_message>
<xml_diff>
--- a/data/info/Journal data archiving policies (as relevant to JDAP).xlsx
+++ b/data/info/Journal data archiving policies (as relevant to JDAP).xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="655" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="532" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="354">
   <si>
     <t>Journal</t>
   </si>
@@ -101,7 +101,7 @@
     <t>American Naturalist</t>
   </si>
   <si>
-    <t>Am. Nat</t>
+    <t>Am. Nat.</t>
   </si>
   <si>
     <t>American Society of Naturalists</t>
@@ -170,6 +170,9 @@
     <t>Springer</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>http://www.springer.com/life+sciences/behavioural/journal/265</t>
   </si>
   <si>
@@ -227,19 +230,7 @@
     <t>http://rsbl.royalsocietypublishing.org/content/author-information</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The policy was between Sep 1, 2014 and before Oct 29, 2014.  The version of the submission guidelines cached by google is dated Oc 29, 2014 and contains the phrase “We require supporting data to be made available prior to publication so that all results are reproducible.“ The old guidelines from Sep 1, 2014 are here: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://web.archive.org/web/20140901235522/http://rsbl.royalsocietypublishing.org/site/misc/information.xhtml</t>
-    </r>
+    <t>The policy was between Sep 1, 2014 and before Oct 29, 2014.  The version of the submission guidelines cached by google is dated Oc 29, 2014 and contains the phrase “We require supporting data to be made available prior to publication so that all results are reproducible.“ The old guidelines from Sep 1, 2014 are here: https://web.archive.org/web/20140901235522/http://rsbl.royalsocietypublishing.org/site/misc/information.xhtml</t>
   </si>
   <si>
     <t>BioRisk</t>
@@ -304,9 +295,6 @@
     <t>Society for Conservation Biology</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>http://onlinelibrary.wiley.com/journal/10.1111/(ISSN)1523-1739/homepage/ForAuthors.html</t>
   </si>
   <si>
@@ -851,6 +839,15 @@
   </si>
   <si>
     <t>PLoS</t>
+  </si>
+  <si>
+    <t>12.10.2014-14.11.2014</t>
+  </si>
+  <si>
+    <t>http://www.plosbiology.org/static/guidelines#datareporting</t>
+  </si>
+  <si>
+    <t>Accrding to archive.org snapshots of the  URL on the left, the policy must have been introduced between Oct 12, 2014 and Nov 14, 2014.</t>
   </si>
   <si>
     <t>PLoS Computational Biology</t>
@@ -1106,7 +1103,7 @@
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
     <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1160,11 +1157,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Abyssinica SIL"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1255,7 +1247,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1308,12 +1300,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1325,14 +1321,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1380,11 +1368,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1407,10 +1395,10 @@
   </sheetPr>
   <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1756,23 +1744,29 @@
       <c r="D15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="H15" s="9"/>
       <c r="I15" s="5"/>
       <c r="J15" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1782,11 +1776,11 @@
     </row>
     <row r="17" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>24</v>
@@ -1799,25 +1793,25 @@
     </row>
     <row r="18" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>56</v>
+      <c r="G18" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>14</v>
@@ -1826,46 +1820,46 @@
         <v>40503</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="13" t="s">
-        <v>64</v>
+      <c r="G19" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="5"/>
       <c r="J19" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19" s="0" t="s">
         <v>66</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1888,14 +1882,14 @@
     </row>
     <row r="21" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1905,17 +1899,17 @@
     </row>
     <row r="22" customFormat="false" ht="88.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="5"/>
@@ -1924,7 +1918,7 @@
     </row>
     <row r="23" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1932,7 +1926,7 @@
         <v>36</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="5"/>
@@ -1941,10 +1935,10 @@
     </row>
     <row r="24" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="4" t="s">
@@ -1956,16 +1950,18 @@
       <c r="F24" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="H24" s="9"/>
       <c r="I24" s="5"/>
       <c r="J24" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1980,7 +1976,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1995,7 +1991,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2010,12 +2006,12 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -2029,24 +2025,26 @@
     </row>
     <row r="29" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G29" s="5"/>
+      <c r="F29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="H29" s="9"/>
       <c r="I29" s="5"/>
       <c r="J29" s="0" t="s">
@@ -2076,7 +2074,7 @@
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>46</v>
@@ -2094,7 +2092,7 @@
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -2109,7 +2107,7 @@
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -2130,7 +2128,7 @@
       <c r="D34" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="16" t="s">
         <v>97</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -2144,7 +2142,7 @@
       <c r="J34" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="K34" s="16" t="s">
+      <c r="K34" s="17" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2167,7 +2165,7 @@
       <c r="F35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="G35" s="18" t="s">
         <v>33</v>
       </c>
       <c r="H35" s="6" t="s">
@@ -2187,7 +2185,7 @@
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -2209,15 +2207,15 @@
         <v>96</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="F37" s="18" t="s">
-        <v>87</v>
+      <c r="F37" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>42</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="19" t="s">
+      <c r="J37" s="15" t="s">
         <v>105</v>
       </c>
       <c r="K37" s="0" t="s">
@@ -2231,7 +2229,7 @@
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -2248,7 +2246,7 @@
         <v>109</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>110</v>
@@ -2284,7 +2282,7 @@
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -2318,7 +2316,7 @@
         <v>116</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>117</v>
@@ -2367,10 +2365,10 @@
         <v>124</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>125</v>
@@ -2449,7 +2447,7 @@
         <v>137</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>138</v>
@@ -2457,7 +2455,7 @@
       <c r="F48" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G48" s="20" t="s">
+      <c r="G48" s="19" t="s">
         <v>139</v>
       </c>
       <c r="H48" s="9"/>
@@ -2476,7 +2474,7 @@
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -2501,7 +2499,7 @@
       <c r="F50" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G50" s="17" t="s">
+      <c r="G50" s="18" t="s">
         <v>147</v>
       </c>
       <c r="H50" s="9"/>
@@ -2551,7 +2549,7 @@
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>154</v>
@@ -2575,7 +2573,7 @@
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -2605,7 +2603,7 @@
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -2741,7 +2739,7 @@
         <v>137</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>177</v>
@@ -2749,7 +2747,7 @@
       <c r="F63" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G63" s="17" t="s">
+      <c r="G63" s="18" t="s">
         <v>178</v>
       </c>
       <c r="H63" s="9"/>
@@ -2790,10 +2788,10 @@
         <v>183</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>154</v>
@@ -2821,7 +2819,7 @@
         <v>137</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>138</v>
@@ -2829,7 +2827,7 @@
       <c r="F66" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G66" s="21" t="s">
+      <c r="G66" s="20" t="s">
         <v>187</v>
       </c>
       <c r="H66" s="9"/>
@@ -2852,7 +2850,7 @@
         <v>192</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>117</v>
@@ -2860,7 +2858,7 @@
       <c r="F67" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G67" s="22" t="s">
+      <c r="G67" s="21" t="s">
         <v>193</v>
       </c>
       <c r="H67" s="6" t="s">
@@ -2921,7 +2919,7 @@
         <v>204</v>
       </c>
       <c r="H69" s="9"/>
-      <c r="I69" s="23"/>
+      <c r="I69" s="22"/>
     </row>
     <row r="70" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
@@ -2945,10 +2943,10 @@
       <c r="G70" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="H70" s="24" t="s">
+      <c r="H70" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I70" s="25" t="n">
+      <c r="I70" s="24" t="n">
         <v>40233</v>
       </c>
       <c r="J70" s="0" t="s">
@@ -2970,7 +2968,7 @@
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="9"/>
-      <c r="I71" s="26"/>
+      <c r="I71" s="25"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
@@ -2987,7 +2985,7 @@
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="G72" s="9" t="s">
         <v>42</v>
@@ -3004,7 +3002,7 @@
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>217</v>
@@ -3032,7 +3030,7 @@
         <v>110</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>42</v>
@@ -3077,12 +3075,12 @@
       <c r="F76" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G76" s="27" t="s">
+      <c r="G76" s="26" t="s">
         <v>227</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="5"/>
-      <c r="J76" s="19" t="s">
+      <c r="J76" s="15" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3094,10 +3092,10 @@
         <v>230</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>117</v>
@@ -3117,7 +3115,7 @@
       <c r="J77" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="K77" s="16" t="s">
+      <c r="K77" s="17" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3127,10 +3125,10 @@
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>203</v>
@@ -3144,7 +3142,7 @@
       <c r="H78" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I78" s="28" t="n">
+      <c r="I78" s="27" t="n">
         <v>40497</v>
       </c>
     </row>
@@ -3156,13 +3154,15 @@
         <v>235</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
+      <c r="F79" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="G79" s="9" t="s">
         <v>42</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>212</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="G85" s="9" t="s">
         <v>42</v>
@@ -3302,7 +3302,7 @@
         <v>252</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>253</v>
@@ -3310,7 +3310,7 @@
       <c r="F86" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G86" s="13" t="s">
+      <c r="G86" s="14" t="s">
         <v>254</v>
       </c>
       <c r="H86" s="9"/>
@@ -3331,7 +3331,7 @@
         <v>258</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
@@ -3358,7 +3358,7 @@
       <c r="F88" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="G88" s="13" t="s">
+      <c r="G88" s="14" t="s">
         <v>262</v>
       </c>
       <c r="H88" s="6" t="s">
@@ -3421,13 +3421,21 @@
       <c r="F91" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G91" s="5"/>
+      <c r="G91" s="20" t="s">
+        <v>270</v>
+      </c>
       <c r="H91" s="9"/>
       <c r="I91" s="5"/>
+      <c r="J91" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="K91" s="0" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="8" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -3442,7 +3450,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="8" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -3457,7 +3465,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="8" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -3472,7 +3480,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="8" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
@@ -3487,7 +3495,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="8" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
@@ -3502,7 +3510,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="8" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
@@ -3517,12 +3525,12 @@
     </row>
     <row r="98" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="8" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="4" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
@@ -3532,7 +3540,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="8" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
@@ -3547,17 +3555,17 @@
     </row>
     <row r="100" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="8" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B100" s="5"/>
       <c r="C100" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="5"/>
@@ -3566,17 +3574,17 @@
     </row>
     <row r="101" customFormat="false" ht="156.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="8" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B101" s="5"/>
       <c r="C101" s="4" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="F101" s="4"/>
       <c r="G101" s="5"/>
@@ -3585,25 +3593,25 @@
     </row>
     <row r="102" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G102" s="27" t="n">
-        <v>2010</v>
+      <c r="G102" s="26" t="s">
+        <v>227</v>
       </c>
       <c r="H102" s="6" t="s">
         <v>14</v>
@@ -3612,17 +3620,17 @@
         <v>40716</v>
       </c>
       <c r="J102" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="8" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
@@ -3632,7 +3640,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="8" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
@@ -3646,35 +3654,37 @@
       <c r="I104" s="5"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="29" t="s">
-        <v>293</v>
+      <c r="A105" s="28" t="s">
+        <v>296</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G105" s="5"/>
+      <c r="G105" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="H105" s="9"/>
       <c r="I105" s="5"/>
       <c r="J105" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="30" t="s">
-        <v>297</v>
+      <c r="A106" s="29" t="s">
+        <v>300</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>22</v>
@@ -3685,17 +3695,20 @@
       <c r="F106" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="G106" s="30" t="s">
+        <v>42</v>
+      </c>
       <c r="H106" s="0"/>
       <c r="J106" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="30" t="s">
-        <v>300</v>
+      <c r="A107" s="29" t="s">
+        <v>303</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D107" s="0" t="s">
         <v>36</v>
@@ -3707,22 +3720,22 @@
         <v>32</v>
       </c>
       <c r="G107" s="31" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="H107" s="0"/>
       <c r="J107" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="K107" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="30" t="s">
-        <v>305</v>
+      <c r="A108" s="29" t="s">
+        <v>308</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D108" s="0" t="s">
         <v>36</v>
@@ -3733,17 +3746,20 @@
       <c r="F108" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="G108" s="30" t="s">
+        <v>42</v>
+      </c>
       <c r="H108" s="0"/>
       <c r="J108" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="30" t="s">
-        <v>308</v>
+      <c r="A109" s="29" t="s">
+        <v>311</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D109" s="0" t="s">
         <v>46</v>
@@ -3752,22 +3768,22 @@
         <v>42</v>
       </c>
       <c r="F109" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G109" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G109" s="30" t="s">
         <v>42</v>
       </c>
       <c r="H109" s="0"/>
       <c r="J109" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="30" t="s">
-        <v>311</v>
+      <c r="A110" s="29" t="s">
+        <v>314</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>46</v>
@@ -3776,22 +3792,22 @@
         <v>42</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G110" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G110" s="30" t="s">
         <v>42</v>
       </c>
       <c r="H110" s="0"/>
       <c r="J110" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="30" t="s">
-        <v>314</v>
+      <c r="A111" s="29" t="s">
+        <v>317</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>22</v>
@@ -3800,22 +3816,22 @@
         <v>42</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G111" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G111" s="30" t="s">
         <v>42</v>
       </c>
       <c r="H111" s="0"/>
       <c r="J111" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="30" t="s">
-        <v>317</v>
+      <c r="A112" s="29" t="s">
+        <v>320</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E112" s="0" t="s">
         <v>253</v>
@@ -3824,113 +3840,113 @@
         <v>32</v>
       </c>
       <c r="G112" s="31" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="I112" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="J112" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="K112" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="30" t="s">
-        <v>323</v>
+      <c r="A113" s="29" t="s">
+        <v>326</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G113" s="32" t="s">
+      <c r="G113" s="30" t="s">
         <v>42</v>
       </c>
       <c r="J113" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="30" t="s">
-        <v>327</v>
+      <c r="A114" s="29" t="s">
+        <v>330</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E114" s="0" t="s">
         <v>42</v>
       </c>
       <c r="F114" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G114" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G114" s="30" t="s">
         <v>42</v>
       </c>
       <c r="J114" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="30" t="s">
-        <v>330</v>
+      <c r="A115" s="29" t="s">
+        <v>333</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="E115" s="12" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="F115" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G115" s="32" t="s">
+      <c r="G115" s="30" t="s">
         <v>42</v>
       </c>
       <c r="J115" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="30" t="s">
-        <v>333</v>
+      <c r="A116" s="29" t="s">
+        <v>336</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="F116" s="5" t="s">
         <v>32</v>
       </c>
       <c r="G116" s="31" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="J116" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="K116" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="30" t="s">
-        <v>339</v>
+      <c r="A117" s="29" t="s">
+        <v>342</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E117" s="12" t="s">
         <v>253</v>
@@ -3939,61 +3955,61 @@
         <v>32</v>
       </c>
       <c r="G117" s="31" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="J117" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="K117" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="30" t="s">
-        <v>344</v>
+      <c r="A118" s="29" t="s">
+        <v>347</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E118" s="0" t="s">
         <v>42</v>
       </c>
       <c r="F118" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G118" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G118" s="30" t="s">
         <v>42</v>
       </c>
       <c r="J118" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="30" t="s">
-        <v>347</v>
+      <c r="A119" s="29" t="s">
+        <v>350</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E119" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F119" s="5" t="s">
         <v>32</v>
       </c>
       <c r="G119" s="31" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="J119" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K19" r:id="rId1" display="https://web.archive.org/web/20140901235522/http://rsbl.royalsocietypublishing.org/site/misc/information.xhtml"/>
+    <hyperlink ref="K19" r:id="rId1" display="The policy was between Sep 1, 2014 and before Oct 29, 2014.  The version of the submission guidelines cached by google is dated Oc 29, 2014 and contains the phrase “We require supporting data to be made available prior to publication so that all results are reproducible.“ The old guidelines from Sep 1, 2014 are here: https://web.archive.org/web/20140901235522/http://rsbl.royalsocietypublishing.org/site/misc/information.xhtml"/>
     <hyperlink ref="J37" r:id="rId2" display="http://esapubs.org/esapubs/DataReg.htm"/>
     <hyperlink ref="J76" r:id="rId3" display="http://mbe.oxfordjournals.org/content/27/3/742.full"/>
   </hyperlinks>

</xml_diff>